<commit_message>
Added OrganisationsImporter for Organisations from excel data.
</commit_message>
<xml_diff>
--- a/tests/fixtures/importer-data.xlsx
+++ b/tests/fixtures/importer-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="types" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="countries-states" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="states-countries" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="countries-states-countries" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="organisations" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
   <si>
     <t xml:space="preserve">blank</t>
   </si>
@@ -172,6 +173,102 @@
   </si>
   <si>
     <t xml:space="preserve">Kebbi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">parent_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fncode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">short_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addr_street</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addr_town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addr_state_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addr_landmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">postal_code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">website_url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date_established</t>
+  </si>
+  <si>
+    <t xml:space="preserve">description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">longitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">latitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">altitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gps_error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-x-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazeltek Solutions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#3 Ansar Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info@hazeltek.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazeltek Media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#5 Post Office Rd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">media@hazeltek.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">080 0000 1111</t>
   </si>
 </sst>
 </file>
@@ -184,11 +281,12 @@
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -211,24 +309,28 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -236,24 +338,28 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF006600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -261,6 +367,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -268,17 +375,27 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -441,7 +558,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -471,6 +588,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -569,7 +690,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
@@ -586,7 +707,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.99"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="11.52"/>
   </cols>
@@ -1184,4 +1305,192 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="9.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="14.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="13.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="10.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="9.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="11.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="2" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="7.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="2" width="6.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="8.23"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="2" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" display="info@hazeltek.com"/>
+    <hyperlink ref="L3" r:id="rId2" display="media@hazeltek.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Rename orgz module to party and use uuid for FK rels
</commit_message>
<xml_diff>
--- a/tests/fixtures/importer-data.xlsx
+++ b/tests/fixtures/importer-data.xlsx
@@ -14,7 +14,7 @@
     <sheet name="countries-states" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="states-countries" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="countries-states-countries" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="organisations" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="organizations" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="80">
   <si>
     <t xml:space="preserve">blank</t>
   </si>
@@ -178,10 +178,7 @@
     <t xml:space="preserve">parent_id</t>
   </si>
   <si>
-    <t xml:space="preserve">identifier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fncode</t>
+    <t xml:space="preserve">subtype</t>
   </si>
   <si>
     <t xml:space="preserve">short_name</t>
@@ -281,7 +278,7 @@
     <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="167" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -304,87 +301,6 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -398,7 +314,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -407,74 +323,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -485,7 +344,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -509,177 +368,53 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -694,7 +429,7 @@
       <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="3.11"/>
@@ -707,7 +442,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="7.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="8.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="11.99"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="17" style="0" width="11.52"/>
   </cols>
@@ -849,7 +584,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="6.29"/>
@@ -908,7 +643,7 @@
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="6.29"/>
@@ -976,7 +711,7 @@
       <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="6.29"/>
@@ -1103,7 +838,7 @@
       <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="6.29"/>
@@ -1189,7 +924,7 @@
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="12.13"/>
@@ -1314,11 +1049,11 @@
   </sheetPr>
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T3" activeCellId="0" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="7.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="7.13"/>
@@ -1329,7 +1064,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="11.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="9.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="9.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="2" width="11.16"/>
@@ -1337,7 +1072,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="2" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="8.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -1346,78 +1081,78 @@
         <v>49</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>34</v>
@@ -1429,7 +1164,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1441,22 +1176,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>34</v>
@@ -1468,10 +1203,10 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>

</xml_diff>

<commit_message>
Add organization types data importer and update organization importer
</commit_message>
<xml_diff>
--- a/tests/fixtures/importer-data.xlsx
+++ b/tests/fixtures/importer-data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="types" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,7 +14,8 @@
     <sheet name="countries-states" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="states-countries" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="countries-states-countries" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="organizations" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="organization-types" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="organizations" sheetId="8" state="visible" r:id="rId9"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="85">
   <si>
     <t xml:space="preserve">blank</t>
   </si>
@@ -175,10 +176,25 @@
     <t xml:space="preserve">Kebbi</t>
   </si>
   <si>
+    <t xml:space="preserve">title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Region</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service-centre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service Centre</t>
+  </si>
+  <si>
     <t xml:space="preserve">parent_id</t>
   </si>
   <si>
-    <t xml:space="preserve">subtype</t>
+    <t xml:space="preserve">type_id</t>
   </si>
   <si>
     <t xml:space="preserve">short_name</t>
@@ -425,8 +441,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O9" activeCellId="0" sqref="O9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -580,8 +596,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -639,7 +655,7 @@
   </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -707,7 +723,7 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F37" activeCellId="0" sqref="F37"/>
     </sheetView>
   </sheetViews>
@@ -834,7 +850,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -920,7 +936,7 @@
   </sheetPr>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1047,10 +1063,62 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T3" activeCellId="0" sqref="T3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1072,87 +1140,87 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="2" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="7.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="2" width="6.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="20" style="2" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>34</v>
@@ -1164,7 +1232,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="8" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1176,22 +1244,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>34</v>
@@ -1203,10 +1271,10 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="8" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>

</xml_diff>

<commit_message>
Refactor imports to use business logic actions
</commit_message>
<xml_diff>
--- a/tests/fixtures/importer-data.xlsx
+++ b/tests/fixtures/importer-data.xlsx
@@ -15,7 +15,8 @@
     <sheet name="states-countries" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="countries-states-countries" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="organization-types" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="organizations" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="organization-types-2" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="organizations" sheetId="9" state="visible" r:id="rId10"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="89">
   <si>
     <t xml:space="preserve">blank</t>
   </si>
@@ -179,16 +180,34 @@
     <t xml:space="preserve">title</t>
   </si>
   <si>
-    <t xml:space="preserve">region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Region</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service-centre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service Centre</t>
+    <t xml:space="preserve">is_root</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sub-branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Branch2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub Branch2</t>
   </si>
   <si>
     <t xml:space="preserve">parent_id</t>
@@ -248,9 +267,6 @@
     <t xml:space="preserve">01</t>
   </si>
   <si>
-    <t xml:space="preserve">hq</t>
-  </si>
-  <si>
     <t xml:space="preserve">HS</t>
   </si>
   <si>
@@ -264,9 +280,6 @@
   </si>
   <si>
     <t xml:space="preserve">0101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">branch</t>
   </si>
   <si>
     <t xml:space="preserve">HSM</t>
@@ -385,7 +398,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -418,6 +431,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -442,7 +463,7 @@
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1063,16 +1084,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="13.02"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1082,21 +1104,36 @@
       <c r="B1" s="3" t="s">
         <v>49</v>
       </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+      <c r="C3" s="9"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1115,10 +1152,80 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="13.02"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:S3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1146,81 +1253,81 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>26</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>34</v>
@@ -1231,8 +1338,8 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="8" t="s">
-        <v>77</v>
+      <c r="L2" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -1244,22 +1351,22 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>34</v>
@@ -1270,11 +1377,11 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="8" t="s">
-        <v>83</v>
+      <c r="L3" s="10" t="s">
+        <v>87</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>

</xml_diff>